<commit_message>
refactor: example runs files
Edits the example run files with new sample names. Updates the docs and
unit tests to match. Removes deprecated example data and documentation.
</commit_message>
<xml_diff>
--- a/inst/extdata/oa_gene_expression_batch1.xlsx
+++ b/inst/extdata/oa_gene_expression_batch1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aidants\_repos\OAtools\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CABEAF4-8D6E-462D-93AE-25D9CCCF9350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0055BBB0-CBC0-4B38-9DF8-905704AF2D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Multicomponent Data" sheetId="4" r:id="rId1"/>
@@ -438,40 +438,40 @@
     <t>Reference Sample</t>
   </si>
   <si>
-    <t>Sample 37</t>
+    <t>Positive Control</t>
   </si>
   <si>
-    <t>Sample 38</t>
+    <t>Sample-101</t>
   </si>
   <si>
-    <t>Sample 39</t>
+    <t>Sample-102</t>
   </si>
   <si>
-    <t>Sample 40</t>
+    <t>Sample-103</t>
   </si>
   <si>
-    <t>Sample 41</t>
+    <t>Sample-104</t>
   </si>
   <si>
-    <t>Sample 42</t>
+    <t>Sample-105</t>
   </si>
   <si>
-    <t>Sample 43</t>
+    <t>Sample-106</t>
   </si>
   <si>
-    <t>Sample 44</t>
+    <t>Sample-107</t>
   </si>
   <si>
-    <t>Sample 45</t>
+    <t>Sample-108</t>
   </si>
   <si>
-    <t>Sample 46</t>
+    <t>Sample-109</t>
   </si>
   <si>
-    <t>Sample 47</t>
+    <t>Sample-110</t>
   </si>
   <si>
-    <t>Positive Control</t>
+    <t>Sample-111</t>
   </si>
 </sst>
 </file>
@@ -54644,8 +54644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A20:R120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54720,7 +54720,7 @@
         <v>124</v>
       </c>
       <c r="D21" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
@@ -54776,7 +54776,7 @@
         <v>124</v>
       </c>
       <c r="D22" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
@@ -54832,7 +54832,7 @@
         <v>124</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E23" t="s">
         <v>14</v>
@@ -54888,7 +54888,7 @@
         <v>124</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E24" t="s">
         <v>14</v>
@@ -54944,7 +54944,7 @@
         <v>124</v>
       </c>
       <c r="D25" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -55000,7 +55000,7 @@
         <v>124</v>
       </c>
       <c r="D26" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E26" t="s">
         <v>15</v>
@@ -55056,7 +55056,7 @@
         <v>124</v>
       </c>
       <c r="D27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>
@@ -55112,7 +55112,7 @@
         <v>124</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E28" t="s">
         <v>16</v>
@@ -55168,7 +55168,7 @@
         <v>124</v>
       </c>
       <c r="D29" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
@@ -55224,7 +55224,7 @@
         <v>124</v>
       </c>
       <c r="D30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E30" t="s">
         <v>13</v>
@@ -55280,7 +55280,7 @@
         <v>124</v>
       </c>
       <c r="D31" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E31" t="s">
         <v>14</v>
@@ -55336,7 +55336,7 @@
         <v>124</v>
       </c>
       <c r="D32" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E32" t="s">
         <v>14</v>
@@ -55392,7 +55392,7 @@
         <v>124</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
@@ -55448,7 +55448,7 @@
         <v>124</v>
       </c>
       <c r="D34" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
@@ -55504,7 +55504,7 @@
         <v>124</v>
       </c>
       <c r="D35" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E35" t="s">
         <v>16</v>
@@ -55560,7 +55560,7 @@
         <v>124</v>
       </c>
       <c r="D36" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E36" t="s">
         <v>16</v>
@@ -55616,7 +55616,7 @@
         <v>124</v>
       </c>
       <c r="D37" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E37" t="s">
         <v>13</v>
@@ -55672,7 +55672,7 @@
         <v>124</v>
       </c>
       <c r="D38" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E38" t="s">
         <v>13</v>
@@ -55728,7 +55728,7 @@
         <v>124</v>
       </c>
       <c r="D39" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E39" t="s">
         <v>14</v>
@@ -55784,7 +55784,7 @@
         <v>124</v>
       </c>
       <c r="D40" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E40" t="s">
         <v>14</v>
@@ -55840,7 +55840,7 @@
         <v>124</v>
       </c>
       <c r="D41" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
@@ -55896,7 +55896,7 @@
         <v>124</v>
       </c>
       <c r="D42" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
@@ -55952,7 +55952,7 @@
         <v>124</v>
       </c>
       <c r="D43" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E43" t="s">
         <v>16</v>
@@ -56008,7 +56008,7 @@
         <v>124</v>
       </c>
       <c r="D44" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E44" t="s">
         <v>16</v>
@@ -56064,7 +56064,7 @@
         <v>124</v>
       </c>
       <c r="D45" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -56120,7 +56120,7 @@
         <v>124</v>
       </c>
       <c r="D46" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E46" t="s">
         <v>13</v>
@@ -56176,7 +56176,7 @@
         <v>124</v>
       </c>
       <c r="D47" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E47" t="s">
         <v>14</v>
@@ -56232,7 +56232,7 @@
         <v>124</v>
       </c>
       <c r="D48" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E48" t="s">
         <v>14</v>
@@ -56288,7 +56288,7 @@
         <v>124</v>
       </c>
       <c r="D49" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
@@ -56344,7 +56344,7 @@
         <v>124</v>
       </c>
       <c r="D50" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
@@ -56400,7 +56400,7 @@
         <v>124</v>
       </c>
       <c r="D51" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E51" t="s">
         <v>16</v>
@@ -56456,7 +56456,7 @@
         <v>124</v>
       </c>
       <c r="D52" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E52" t="s">
         <v>16</v>
@@ -56512,7 +56512,7 @@
         <v>124</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E53" t="s">
         <v>13</v>
@@ -56568,7 +56568,7 @@
         <v>124</v>
       </c>
       <c r="D54" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E54" t="s">
         <v>13</v>
@@ -56624,7 +56624,7 @@
         <v>124</v>
       </c>
       <c r="D55" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
@@ -56680,7 +56680,7 @@
         <v>124</v>
       </c>
       <c r="D56" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
@@ -56736,7 +56736,7 @@
         <v>124</v>
       </c>
       <c r="D57" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E57" t="s">
         <v>15</v>
@@ -56792,7 +56792,7 @@
         <v>124</v>
       </c>
       <c r="D58" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E58" t="s">
         <v>15</v>
@@ -56848,7 +56848,7 @@
         <v>124</v>
       </c>
       <c r="D59" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E59" t="s">
         <v>16</v>
@@ -56904,7 +56904,7 @@
         <v>124</v>
       </c>
       <c r="D60" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E60" t="s">
         <v>16</v>
@@ -56960,7 +56960,7 @@
         <v>124</v>
       </c>
       <c r="D61" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
@@ -57016,7 +57016,7 @@
         <v>124</v>
       </c>
       <c r="D62" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>
@@ -57072,7 +57072,7 @@
         <v>124</v>
       </c>
       <c r="D63" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E63" t="s">
         <v>14</v>
@@ -57128,7 +57128,7 @@
         <v>124</v>
       </c>
       <c r="D64" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E64" t="s">
         <v>14</v>
@@ -57184,7 +57184,7 @@
         <v>124</v>
       </c>
       <c r="D65" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
@@ -57240,7 +57240,7 @@
         <v>124</v>
       </c>
       <c r="D66" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E66" t="s">
         <v>15</v>
@@ -57296,7 +57296,7 @@
         <v>124</v>
       </c>
       <c r="D67" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E67" t="s">
         <v>16</v>
@@ -57352,7 +57352,7 @@
         <v>124</v>
       </c>
       <c r="D68" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E68" t="s">
         <v>16</v>
@@ -57408,7 +57408,7 @@
         <v>124</v>
       </c>
       <c r="D69" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
@@ -57464,7 +57464,7 @@
         <v>124</v>
       </c>
       <c r="D70" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
@@ -57520,7 +57520,7 @@
         <v>124</v>
       </c>
       <c r="D71" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E71" t="s">
         <v>14</v>
@@ -57576,7 +57576,7 @@
         <v>124</v>
       </c>
       <c r="D72" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E72" t="s">
         <v>14</v>
@@ -57632,7 +57632,7 @@
         <v>124</v>
       </c>
       <c r="D73" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
@@ -57688,7 +57688,7 @@
         <v>124</v>
       </c>
       <c r="D74" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E74" t="s">
         <v>15</v>
@@ -57744,7 +57744,7 @@
         <v>124</v>
       </c>
       <c r="D75" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E75" t="s">
         <v>16</v>
@@ -57800,7 +57800,7 @@
         <v>124</v>
       </c>
       <c r="D76" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E76" t="s">
         <v>16</v>
@@ -57856,7 +57856,7 @@
         <v>124</v>
       </c>
       <c r="D77" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E77" t="s">
         <v>13</v>
@@ -57912,7 +57912,7 @@
         <v>124</v>
       </c>
       <c r="D78" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E78" t="s">
         <v>13</v>
@@ -57968,7 +57968,7 @@
         <v>124</v>
       </c>
       <c r="D79" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E79" t="s">
         <v>14</v>
@@ -58024,7 +58024,7 @@
         <v>124</v>
       </c>
       <c r="D80" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E80" t="s">
         <v>14</v>
@@ -58080,7 +58080,7 @@
         <v>124</v>
       </c>
       <c r="D81" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
@@ -58136,7 +58136,7 @@
         <v>124</v>
       </c>
       <c r="D82" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E82" t="s">
         <v>15</v>
@@ -58192,7 +58192,7 @@
         <v>124</v>
       </c>
       <c r="D83" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E83" t="s">
         <v>16</v>
@@ -58248,7 +58248,7 @@
         <v>124</v>
       </c>
       <c r="D84" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E84" t="s">
         <v>16</v>
@@ -58304,7 +58304,7 @@
         <v>124</v>
       </c>
       <c r="D85" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E85" t="s">
         <v>13</v>
@@ -58360,7 +58360,7 @@
         <v>124</v>
       </c>
       <c r="D86" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E86" t="s">
         <v>13</v>
@@ -58416,7 +58416,7 @@
         <v>124</v>
       </c>
       <c r="D87" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E87" t="s">
         <v>14</v>
@@ -58472,7 +58472,7 @@
         <v>124</v>
       </c>
       <c r="D88" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E88" t="s">
         <v>14</v>
@@ -58528,7 +58528,7 @@
         <v>124</v>
       </c>
       <c r="D89" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
@@ -58584,7 +58584,7 @@
         <v>124</v>
       </c>
       <c r="D90" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E90" t="s">
         <v>15</v>
@@ -58640,7 +58640,7 @@
         <v>124</v>
       </c>
       <c r="D91" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E91" t="s">
         <v>16</v>
@@ -58696,7 +58696,7 @@
         <v>124</v>
       </c>
       <c r="D92" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E92" t="s">
         <v>16</v>
@@ -58752,7 +58752,7 @@
         <v>124</v>
       </c>
       <c r="D93" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E93" t="s">
         <v>13</v>
@@ -58808,7 +58808,7 @@
         <v>124</v>
       </c>
       <c r="D94" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E94" t="s">
         <v>13</v>
@@ -58864,7 +58864,7 @@
         <v>124</v>
       </c>
       <c r="D95" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E95" t="s">
         <v>14</v>
@@ -58920,7 +58920,7 @@
         <v>124</v>
       </c>
       <c r="D96" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E96" t="s">
         <v>14</v>
@@ -58976,7 +58976,7 @@
         <v>124</v>
       </c>
       <c r="D97" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E97" t="s">
         <v>15</v>
@@ -59032,7 +59032,7 @@
         <v>124</v>
       </c>
       <c r="D98" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E98" t="s">
         <v>15</v>
@@ -59088,7 +59088,7 @@
         <v>124</v>
       </c>
       <c r="D99" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E99" t="s">
         <v>16</v>
@@ -59144,7 +59144,7 @@
         <v>124</v>
       </c>
       <c r="D100" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E100" t="s">
         <v>16</v>
@@ -59200,7 +59200,7 @@
         <v>124</v>
       </c>
       <c r="D101" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E101" t="s">
         <v>13</v>
@@ -59256,7 +59256,7 @@
         <v>124</v>
       </c>
       <c r="D102" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E102" t="s">
         <v>13</v>
@@ -59312,7 +59312,7 @@
         <v>124</v>
       </c>
       <c r="D103" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E103" t="s">
         <v>14</v>
@@ -59368,7 +59368,7 @@
         <v>124</v>
       </c>
       <c r="D104" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E104" t="s">
         <v>14</v>
@@ -59424,7 +59424,7 @@
         <v>124</v>
       </c>
       <c r="D105" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E105" t="s">
         <v>15</v>
@@ -59480,7 +59480,7 @@
         <v>124</v>
       </c>
       <c r="D106" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E106" t="s">
         <v>15</v>
@@ -59536,7 +59536,7 @@
         <v>124</v>
       </c>
       <c r="D107" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E107" t="s">
         <v>16</v>
@@ -59592,7 +59592,7 @@
         <v>124</v>
       </c>
       <c r="D108" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E108" t="s">
         <v>16</v>
@@ -59648,7 +59648,7 @@
         <v>124</v>
       </c>
       <c r="D109" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E109" t="s">
         <v>13</v>
@@ -59704,7 +59704,7 @@
         <v>124</v>
       </c>
       <c r="D110" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E110" t="s">
         <v>13</v>
@@ -59760,7 +59760,7 @@
         <v>124</v>
       </c>
       <c r="D111" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E111" t="s">
         <v>14</v>
@@ -59816,7 +59816,7 @@
         <v>124</v>
       </c>
       <c r="D112" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E112" t="s">
         <v>14</v>
@@ -59872,7 +59872,7 @@
         <v>124</v>
       </c>
       <c r="D113" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E113" t="s">
         <v>15</v>
@@ -59928,7 +59928,7 @@
         <v>124</v>
       </c>
       <c r="D114" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E114" t="s">
         <v>15</v>
@@ -59984,7 +59984,7 @@
         <v>124</v>
       </c>
       <c r="D115" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E115" t="s">
         <v>16</v>
@@ -60040,7 +60040,7 @@
         <v>124</v>
       </c>
       <c r="D116" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E116" t="s">
         <v>16</v>
@@ -60114,7 +60114,7 @@
         <v>136</v>
       </c>
       <c r="B120" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>